<commit_message>
fix([Global]): Copy all essential files from mob jynew
</commit_message>
<xml_diff>
--- a/Configs/游戏设置.xlsx
+++ b/Configs/游戏设置.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jynew\jyx2\Assets\Mods\SAMPLE\Configs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jynew\jyx2\Assets\Mods\JYX2\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6C49FC-909B-4E0E-BAFA-948890B5C3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EB4E20-B7E6-4C33-AB5C-8F46C3E14307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2960" windowWidth="19140" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="1990" windowWidth="19140" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="战斗数据" sheetId="1" r:id="rId1"/>
@@ -709,13 +709,13 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="65.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.1796875" customWidth="1"/>
@@ -743,6 +743,10 @@
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -891,7 +895,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>24</v>
@@ -1073,7 +1077,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="1">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>50</v>
@@ -1115,7 +1119,7 @@
         <v>55</v>
       </c>
       <c r="C29" s="1">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>56</v>
@@ -1149,7 +1153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -1159,11 +1163,11 @@
       <c r="C32" s="1">
         <v>6</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -1173,11 +1177,11 @@
       <c r="C33" s="1">
         <v>10</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -1187,7 +1191,7 @@
       <c r="C34" s="1">
         <v>3</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="1" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>